<commit_message>
implemented the excel database for adding and deleting products
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_0e9fca7" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,7 +25,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +47,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +72,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,13 +435,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -460,6 +470,21 @@
         </is>
       </c>
       <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>28/01/2025</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
         </is>

</xml_diff>

<commit_message>
added confimation alert to delete function
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_0e9fca7" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,6 +29,9 @@
       <b val="1"/>
       <sz val="11"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -38,7 +41,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -61,13 +64,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
added id to get_productdata and fixxed the error (but without saving the description)
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_0e9fca7" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9c650ad" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_c4955e1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_2b6fb5b" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -520,4 +522,106 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>109</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10/02/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SanDisk SSD PLUS 1TB Internal SSD - SATA III 6 Gb/s</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>695</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>10/02/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>John Hardy Women's Legends Naga Gold &amp; Silver Dragon Station Chain Bracelet</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
switched the display of the urls to displaying the product name (deletion still by url)
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -9,8 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_0e9fca7" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9c650ad" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_c4955e1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_2b6fb5b" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_2b6fb5b" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9037e8e" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -557,7 +557,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>109</v>
+        <v>695</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -566,7 +566,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SanDisk SSD PLUS 1TB Internal SSD - SATA III 6 Gb/s</t>
+          <t>John Hardy Women's Legends Naga Gold &amp; Silver Dragon Station Chain Bracelet</t>
         </is>
       </c>
     </row>
@@ -608,7 +608,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>695</v>
+        <v>109.95</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -617,7 +617,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>John Hardy Women's Legends Naga Gold &amp; Silver Dragon Station Chain Bracelet</t>
+          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[ Matti-Dev ] Removed debugging statements
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_0e9fca7" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9c650ad" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9c650ad" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_ae0513b" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -453,7 +453,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22.3</v>
+        <v>55.99</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -462,7 +462,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+          <t>Mens Cotton Jacket</t>
         </is>
       </c>
     </row>
@@ -504,16 +504,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>55.99</v>
+        <v>15.99</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>04/02/2025</t>
+          <t>12/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mens Cotton Jacket</t>
+          <t>Mens Casual Slim Fit</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixxed some minor errors
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -7,10 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_0e9fca7" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9c650ad" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_2b6fb5b" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9037e8e" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_cd22e94" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_49d69c3" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,22 +447,42 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>product</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22.3</v>
+        <v>695</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>04/02/2025</t>
+          <t>16/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+          <t>John Hardy Women's Legends Naga Gold &amp; Silver Dragon Station Chain Bracelet</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>From our Legends Collection, the Naga was inspired by the mythical water dragon that protects the ocean's pearl. Wear facing inward to be bestowed with love and abundance, or outward for protection.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ID_cd22e94</t>
         </is>
       </c>
     </row>
@@ -479,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,124 +518,67 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>product</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>55.99</v>
+        <v>9.99</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>04/02/2025</t>
+          <t>16/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mens Cotton Jacket</t>
+          <t>White Gold Plated Princess</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Classic Created Wedding Engagement Solitaire Diamond Promise Ring for Her. Gifts to spoil your love more for Engagement, Wedding, Anniversary, Valentine's Day...</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ID_49d69c3</t>
         </is>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>product</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>695</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>10/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>John Hardy Women's Legends Naga Gold &amp; Silver Dragon Station Chain Bracelet</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>product</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>109.95</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>10/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>16/02/2025</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>White Gold Plated Princess</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Classic Created Wedding Engagement Solitaire Diamond Promise Ring for Her. Gifts to spoil your love more for Engagement, Wedding, Anniversary, Valentine's Day...</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ID_49d69c3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[ Matti-Dev ] Little preparations + Added one requested import in views.py
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_7e0f17b" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_dda333c" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_ca64249" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,6 +427,198 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>109.95</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>15/02/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Your perfect pack for everyday use and walks in the forest. Stash your laptop (up to 15 inches) in the padded sleeve, your everyday</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ID_7e0f17b</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>109.95</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>15/02/2025</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Your perfect pack for everyday use and walks in the forest. Stash your laptop (up to 15 inches) in the padded sleeve, your everyday</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ID_7e0f17b</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>15/02/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ID_dda333c</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>15/02/2025</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ID_dda333c</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -462,26 +656,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>109.95</v>
+        <v>109</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14/02/2025</t>
+          <t>15/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
+          <t>SanDisk SSD PLUS 1TB Internal SSD - SATA III 6 Gb/s</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Your perfect pack for everyday use and walks in the forest. Stash your laptop (up to 15 inches) in the padded sleeve, your everyday</t>
+          <t>Easy upgrade for faster boot up, shutdown, application load and response (As compared to 5400 RPM SATA 2.5” hard drive; Based on published specifications and internal benchmarking tests using PCMark vantage scores) Boosts burst write performance, making it ideal for typical PC workloads The perfect balance of performance and reliability Read/write speeds of up to 535MB/s/450MB/s (Based on internal testing; Performance may vary depending upon drive capacity, host device, OS and application.)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ID_7e0f17b</t>
+          <t>ID_ca64249</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[ Matti-Dev ] Little styling change in create.html
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -10,6 +10,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_7e0f17b" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_dda333c" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_ca64249" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_867f88d" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_49d69c3" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -682,4 +684,146 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>15.99</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>17/02/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Mens Casual Slim Fit</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>The color could be slightly different between on the screen and in practice. / Please note that body builds vary by person, therefore, detailed size information should be reviewed below on the product description.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ID_867f88d</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>17/02/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>White Gold Plated Princess</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Classic Created Wedding Engagement Solitaire Diamond Promise Ring for Her. Gifts to spoil your love more for Engagement, Wedding, Anniversary, Valentine's Day...</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ID_49d69c3</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[ Main (without merge) ] Finished and integrated the GET functions
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -8,8 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_7e0f17b" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_dda333c" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_ca64249" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_03f327c" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +467,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>15/02/2025</t>
+          <t>17/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -482,31 +481,6 @@
         </is>
       </c>
       <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_7e0f17b</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>109.95</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>15/02/2025</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Your perfect pack for everyday use and walks in the forest. Stash your laptop (up to 15 inches) in the padded sleeve, your everyday</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
         <is>
           <t>ID_7e0f17b</t>
         </is>
@@ -518,102 +492,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>15/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_dda333c</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>15/02/2025</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ID_dda333c</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -656,26 +534,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>109</v>
+        <v>55.99</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>15/02/2025</t>
+          <t>17/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SanDisk SSD PLUS 1TB Internal SSD - SATA III 6 Gb/s</t>
+          <t>Mens Cotton Jacket</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Easy upgrade for faster boot up, shutdown, application load and response (As compared to 5400 RPM SATA 2.5” hard drive; Based on published specifications and internal benchmarking tests using PCMark vantage scores) Boosts burst write performance, making it ideal for typical PC workloads The perfect balance of performance and reliability Read/write speeds of up to 535MB/s/450MB/s (Based on internal testing; Performance may vary depending upon drive capacity, host device, OS and application.)</t>
+          <t>great outerwear jackets for Spring/Autumn/Winter, suitable for many occasions, such as working, hiking, camping, mountain/rock climbing, cycling, traveling or other outdoors. Good gift choice for you or your family member. A warm hearted love to Father, husband or son in this thanksgiving or Christmas Day.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ID_ca64249</t>
+          <t>ID_03f327c</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added button that deletes products directly out of the list
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_cd22e94" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_49d69c3" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -467,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16/02/2025</t>
+          <t>17/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,102 +482,6 @@
       <c r="E2" t="inlineStr">
         <is>
           <t>ID_cd22e94</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>9.99</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>16/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>White Gold Plated Princess</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Classic Created Wedding Engagement Solitaire Diamond Promise Ring for Her. Gifts to spoil your love more for Engagement, Wedding, Anniversary, Valentine's Day...</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_49d69c3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>9.99</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>16/02/2025</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>White Gold Plated Princess</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Classic Created Wedding Engagement Solitaire Diamond Promise Ring for Her. Gifts to spoil your love more for Engagement, Wedding, Anniversary, Valentine's Day...</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ID_49d69c3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[ Matti-Dev ] Little changes
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -8,10 +8,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_7e0f17b" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_dda333c" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_ca64249" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_867f88d" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_49d69c3" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,198 +425,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>109.95</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>15/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Your perfect pack for everyday use and walks in the forest. Stash your laptop (up to 15 inches) in the padded sleeve, your everyday</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_7e0f17b</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>109.95</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>15/02/2025</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Your perfect pack for everyday use and walks in the forest. Stash your laptop (up to 15 inches) in the padded sleeve, your everyday</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ID_7e0f17b</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>15/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_dda333c</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>15/02/2025</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ID_dda333c</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -658,168 +462,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>109</v>
+        <v>109.95</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>15/02/2025</t>
+          <t>17/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SanDisk SSD PLUS 1TB Internal SSD - SATA III 6 Gb/s</t>
+          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Easy upgrade for faster boot up, shutdown, application load and response (As compared to 5400 RPM SATA 2.5” hard drive; Based on published specifications and internal benchmarking tests using PCMark vantage scores) Boosts burst write performance, making it ideal for typical PC workloads The perfect balance of performance and reliability Read/write speeds of up to 535MB/s/450MB/s (Based on internal testing; Performance may vary depending upon drive capacity, host device, OS and application.)</t>
+          <t>Your perfect pack for everyday use and walks in the forest. Stash your laptop (up to 15 inches) in the padded sleeve, your everyday</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ID_ca64249</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>15.99</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>17/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Mens Casual Slim Fit</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>The color could be slightly different between on the screen and in practice. / Please note that body builds vary by person, therefore, detailed size information should be reviewed below on the product description.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_867f88d</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>9.99</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>17/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>White Gold Plated Princess</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Classic Created Wedding Engagement Solitaire Diamond Promise Ring for Her. Gifts to spoil your love more for Engagement, Wedding, Anniversary, Valentine's Day...</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_49d69c3</t>
+          <t>ID_7e0f17b</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[ Matti-Dev ] Adjusted Styling for the Delete Button of the create Page
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_7e0f17b" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_867f88d" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_03f327c" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,26 +463,97 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>109.95</v>
+        <v>15.99</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>17/02/2025</t>
+          <t>18/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
+          <t>Mens Casual Slim Fit</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Your perfect pack for everyday use and walks in the forest. Stash your laptop (up to 15 inches) in the padded sleeve, your everyday</t>
+          <t>The color could be slightly different between on the screen and in practice. / Please note that body builds vary by person, therefore, detailed size information should be reviewed below on the product description.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ID_7e0f17b</t>
+          <t>ID_867f88d</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>55.99</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>18/02/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Mens Cotton Jacket</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>great outerwear jackets for Spring/Autumn/Winter, suitable for many occasions, such as working, hiking, camping, mountain/rock climbing, cycling, traveling or other outdoors. Good gift choice for you or your family member. A warm hearted love to Father, husband or son in this thanksgiving or Christmas Day.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ID_03f327c</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[ Matti-Dev ] FINAL feature added; Charts -> few adjustments
In the dashboard and home page are now all price charts displayed as intented. I have changed the stylings for better readability of the chart information. At first, the plots where encoded in the wrong backend mode, I changed it to 'AGG' along the matplotlib docs to fix it.
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -7,8 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_7e0f17b" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_03f327c" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_dda333c" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_867f88d" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9a601b4" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -463,26 +464,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>109.95</v>
+        <v>22.3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>20/02/2025</t>
+          <t>21/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Your perfect pack for everyday use and walks in the forest. Stash your laptop (up to 15 inches) in the padded sleeve, your everyday</t>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ID_7e0f17b</t>
+          <t>ID_dda333c</t>
         </is>
       </c>
     </row>
@@ -534,26 +535,97 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>55.99</v>
+        <v>15.99</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>20/02/2025</t>
+          <t>21/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mens Cotton Jacket</t>
+          <t>Mens Casual Slim Fit</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>great outerwear jackets for Spring/Autumn/Winter, suitable for many occasions, such as working, hiking, camping, mountain/rock climbing, cycling, traveling or other outdoors. Good gift choice for you or your family member. A warm hearted love to Father, husband or son in this thanksgiving or Christmas Day.</t>
+          <t>The color could be slightly different between on the screen and in practice. / Please note that body builds vary by person, therefore, detailed size information should be reviewed below on the product description.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ID_03f327c</t>
+          <t>ID_867f88d</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>29.95</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>21/02/2025</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Lock and Love Women's Removable Hooded Faux Leather Moto Biker Jacket</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>100% POLYURETHANE(shell) 100% POLYESTER(lining) 75% POLYESTER 25% COTTON (SWEATER), Faux leather material for style and comfort / 2 pockets of front, 2-For-One Hooded denim style faux leather jacket, Button detail on waist / Detail stitching at sides, HAND WASH ONLY / DO NOT BLEACH / LINE DRY / DO NOT IRON</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ID_9a601b4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[ Main (without merge) ] Clean Up for better Styling
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -7,9 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_dda333c" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_867f88d" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9a601b4" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_867f88d" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9a601b4" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -464,7 +463,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22.3</v>
+        <v>15.99</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -473,17 +472,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+          <t>Mens Casual Slim Fit</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+          <t>The color could be slightly different between on the screen and in practice. / Please note that body builds vary by person, therefore, detailed size information should be reviewed below on the product description.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ID_dda333c</t>
+          <t>ID_867f88d</t>
         </is>
       </c>
     </row>
@@ -535,77 +534,6 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15.99</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>21/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Mens Casual Slim Fit</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>The color could be slightly different between on the screen and in practice. / Please note that body builds vary by person, therefore, detailed size information should be reviewed below on the product description.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_867f88d</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
         <v>29.95</v>
       </c>
       <c r="B2" t="inlineStr">

</xml_diff>

<commit_message>
changed the utils to allow an accuracte prediction if values are given
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -1,38 +1,106 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Studium\Pythonprojekt\Amazon-Price-Tracker\amazon_price_tracker_app\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46A4009-5341-4775-910C-30E3B3D04437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_867f88d" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9a601b4" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ID_867f88d" sheetId="1" r:id="rId1"/>
+    <sheet name="ID_9a601b4" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>21/02/2025</t>
+  </si>
+  <si>
+    <t>Mens Casual Slim Fit</t>
+  </si>
+  <si>
+    <t>The color could be slightly different between on the screen and in practice. / Please note that body builds vary by person, therefore, detailed size information should be reviewed below on the product description.</t>
+  </si>
+  <si>
+    <t>ID_867f88d</t>
+  </si>
+  <si>
+    <t>Lock and Love Women's Removable Hooded Faux Leather Moto Biker Jacket</t>
+  </si>
+  <si>
+    <t>100% POLYURETHANE(shell) 100% POLYESTER(lining) 75% POLYESTER 25% COTTON (SWEATER), Faux leather material for style and comfort / 2 pockets of front, 2-For-One Hooded denim style faux leather jacket, Button detail on waist / Detail stitching at sides, HAND WASH ONLY / DO NOT BLEACH / LINE DRY / DO NOT IRON</t>
+  </si>
+  <si>
+    <t>ID_9a601b4</t>
+  </si>
+  <si>
+    <t>22/02/2025</t>
+  </si>
+  <si>
+    <t>23/02/2026</t>
+  </si>
+  <si>
+    <t>24/02/2027</t>
+  </si>
+  <si>
+    <t>25/02/2028</t>
+  </si>
+  <si>
+    <t>26/02/2029</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,93 +115,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -421,140 +440,183 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>15.99</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>21/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Mens Casual Slim Fit</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>The color could be slightly different between on the screen and in practice. / Please note that body builds vary by person, therefore, detailed size information should be reviewed below on the product description.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_867f88d</t>
-        </is>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>16.7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>14.2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>16.3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>29.95</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>21/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Lock and Love Women's Removable Hooded Faux Leather Moto Biker Jacket</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>100% POLYURETHANE(shell) 100% POLYESTER(lining) 75% POLYESTER 25% COTTON (SWEATER), Faux leather material for style and comfort / 2 pockets of front, 2-For-One Hooded denim style faux leather jacket, Button detail on waist / Detail stitching at sides, HAND WASH ONLY / DO NOT BLEACH / LINE DRY / DO NOT IRON</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_9a601b4</t>
-        </is>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ Main (without merge) ] Little deletions
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_867f88d" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_9a601b4" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_dda333c" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -463,97 +462,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15.99</v>
+        <v>22.3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21/02/2025</t>
+          <t>23/02/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mens Casual Slim Fit</t>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>The color could be slightly different between on the screen and in practice. / Please note that body builds vary by person, therefore, detailed size information should be reviewed below on the product description.</t>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ID_867f88d</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>29.95</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>21/02/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Lock and Love Women's Removable Hooded Faux Leather Moto Biker Jacket</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>100% POLYURETHANE(shell) 100% POLYESTER(lining) 75% POLYESTER 25% COTTON (SWEATER), Faux leather material for style and comfort / 2 pockets of front, 2-For-One Hooded denim style faux leather jacket, Button detail on waist / Detail stitching at sides, HAND WASH ONLY / DO NOT BLEACH / LINE DRY / DO NOT IRON</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ID_9a601b4</t>
+          <t>ID_dda333c</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[ Main (without merge) ] More realistic price prediction
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -4,26 +4,49 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_dda333c" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_7d50ff2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Cambria"/>
+      <charset val="1"/>
+      <family val="0"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -37,7 +60,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -50,21 +73,51 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -137,41 +190,41 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="1f497d"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="eeece1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4f81bd"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="c0504d"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="9bbb59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="8064a2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4bacc6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="f79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0000ff"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -179,243 +232,135 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
-                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
-                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
-                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -425,7 +370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,27 +379,273 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>ID_dda333c</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>ID_dda333c</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>ID_dda333c</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>ID_dda333c</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>ID_dda333c</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>ID_dda333c</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+        </is>
+      </c>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>ID_dda333c</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+        </is>
+      </c>
+      <c r="E9" s="5" t="inlineStr">
+        <is>
+          <t>ID_dda333c</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -462,7 +653,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22.3</v>
+        <v>168</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -471,17 +662,192 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
+          <t xml:space="preserve">Solid Gold Petite Micropave </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
+          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ID_dda333c</t>
+          <t>ID_7d50ff2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>168</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solid Gold Petite Micropave </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ID_7d50ff2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>168</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solid Gold Petite Micropave </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ID_7d50ff2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>168</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solid Gold Petite Micropave </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ID_7d50ff2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>168</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solid Gold Petite Micropave </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ID_7d50ff2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>168</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solid Gold Petite Micropave </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ID_7d50ff2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>168</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solid Gold Petite Micropave </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ID_7d50ff2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>168</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>23/02/2025</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solid Gold Petite Micropave </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ID_7d50ff2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixxed display in main view, fixxed prediction
</commit_message>
<xml_diff>
--- a/amazon_price_tracker_app/data/amazon_product_data.xlsx
+++ b/amazon_price_tracker_app/data/amazon_product_data.xlsx
@@ -2,23 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_dda333c" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_7d50ff2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ID_49d69c3" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -27,24 +26,12 @@
       <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Cambria"/>
-      <charset val="1"/>
-      <family val="0"/>
+      <name val="Calibri"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -60,7 +47,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -69,10 +56,33 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -82,42 +92,25 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -190,41 +183,41 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -232,12 +225,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -266,7 +259,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -287,7 +280,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -338,7 +331,7 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -356,11 +349,13 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -370,13 +365,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
@@ -406,200 +401,150 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="n">
+      <c r="A2" t="n">
         <v>22.3</v>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>23/02/2025</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>ID_dda333c</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="A3" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>24/02/2025</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>ID_dda333c</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n">
+      <c r="A4" t="n">
         <v>25</v>
       </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>25/02/2025</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>ID_dda333c</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>30.3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>26/02/2025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>ID_dda333c</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n">
+      <c r="A6" t="n">
         <v>50</v>
       </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>27/02/2025</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>ID_dda333c</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
+      <c r="A7" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>28/02/2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
         </is>
       </c>
-      <c r="E7" s="5" t="inlineStr">
-        <is>
-          <t>ID_dda333c</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
-        </is>
-      </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
-        </is>
-      </c>
-      <c r="E8" s="5" t="inlineStr">
-        <is>
-          <t>ID_dda333c</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mens Casual Premium Slim Fit T-Shirts </t>
-        </is>
-      </c>
-      <c r="D9" s="5" t="inlineStr">
-        <is>
-          <t>Slim-fitting style, contrast raglan long sleeve, three-button henley placket, light weight &amp; soft fabric for breathable and comfortable wearing. And Solid stitched shirts with round neck made for durability and a great fit for casual fashion wear and diehard baseball fans. The Henley style round neckline includes a three-button placket.</t>
-        </is>
-      </c>
-      <c r="E9" s="5" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>ID_dda333c</t>
         </is>
@@ -616,7 +561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,27 +570,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -653,7 +598,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>168</v>
+        <v>9.99</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -662,192 +607,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Solid Gold Petite Micropave </t>
+          <t>White Gold Plated Princess</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
+          <t>Classic Created Wedding Engagement Solitaire Diamond Promise Ring for Her. Gifts to spoil your love more for Engagement, Wedding, Anniversary, Valentine's Day...</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ID_7d50ff2</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>168</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Solid Gold Petite Micropave </t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ID_7d50ff2</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>168</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Solid Gold Petite Micropave </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>ID_7d50ff2</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>168</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Solid Gold Petite Micropave </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>ID_7d50ff2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>168</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Solid Gold Petite Micropave </t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ID_7d50ff2</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>168</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Solid Gold Petite Micropave </t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ID_7d50ff2</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>168</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Solid Gold Petite Micropave </t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ID_7d50ff2</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>168</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>23/02/2025</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Solid Gold Petite Micropave </t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Satisfaction Guaranteed. Return or exchange any order within 30 days.Designed and sold by Hafeez Center in the United States. Satisfaction Guaranteed. Return or exchange any order within 30 days.</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>ID_7d50ff2</t>
+          <t>ID_49d69c3</t>
         </is>
       </c>
     </row>

</xml_diff>